<commit_message>
borrado registro horas viejo
</commit_message>
<xml_diff>
--- a/RegistroHoras.xlsx
+++ b/RegistroHoras.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silvia\Desktop\TISJ\Prog App\Laboratorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silvia\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DCB6C5B-924A-49B2-8F52-F53E340E8004}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC345F2-5247-4B7C-A688-66A09A480A41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1916,7 +1916,7 @@
   <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2085,13 +2085,21 @@
         <f t="shared" ref="K3:K10" si="0">SUM(G3:J3)</f>
         <v>2</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="11"/>
+      <c r="L3" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="M3" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="N3" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="O3" s="11">
+        <v>0.5</v>
+      </c>
       <c r="P3" s="12">
         <f t="shared" ref="P3:P10" si="1">SUM(L3:O3)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q3" s="13"/>
       <c r="R3" s="10"/>
@@ -2102,8 +2110,8 @@
         <v>0</v>
       </c>
       <c r="V3" s="14">
-        <f t="shared" ref="V3:V10" si="3">SUM(U3,P3,F3)</f>
-        <v>2</v>
+        <f>SUM(U3,P3,F3,K3)</f>
+        <v>6</v>
       </c>
       <c r="W3" s="2"/>
       <c r="X3" s="3"/>
@@ -2134,11 +2142,15 @@
       <c r="H4" s="17">
         <v>1.5</v>
       </c>
-      <c r="I4" s="17"/>
-      <c r="J4" s="18"/>
+      <c r="I4" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="J4" s="18">
+        <v>1</v>
+      </c>
       <c r="K4" s="19">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="L4" s="20"/>
       <c r="M4" s="17"/>
@@ -2157,8 +2169,8 @@
         <v>0</v>
       </c>
       <c r="V4" s="21">
-        <f t="shared" si="3"/>
-        <v>6.25</v>
+        <f>SUM(U4,P4,F4,K4)</f>
+        <v>10.25</v>
       </c>
       <c r="W4" s="2"/>
       <c r="X4" s="3"/>
@@ -2174,16 +2186,22 @@
       <c r="D5" s="17"/>
       <c r="E5" s="18"/>
       <c r="F5" s="19">
-        <f t="shared" ref="F5:F10" si="4">SUM(B5:E5)</f>
+        <f t="shared" ref="F5:F10" si="3">SUM(B5:E5)</f>
         <v>0</v>
       </c>
       <c r="G5" s="20"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="18"/>
+      <c r="H5" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="J5" s="18">
+        <v>1.5</v>
+      </c>
       <c r="K5" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="L5" s="20"/>
       <c r="M5" s="17"/>
@@ -2202,8 +2220,8 @@
         <v>0</v>
       </c>
       <c r="V5" s="21">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>SUM(U5,K5,P5,F5)</f>
+        <v>3.5</v>
       </c>
       <c r="W5" s="2"/>
       <c r="X5" s="3"/>
@@ -2219,7 +2237,7 @@
       <c r="D6" s="17"/>
       <c r="E6" s="18"/>
       <c r="F6" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G6" s="20"/>
@@ -2231,12 +2249,18 @@
         <v>0</v>
       </c>
       <c r="L6" s="20"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="18"/>
+      <c r="M6" s="17">
+        <v>2</v>
+      </c>
+      <c r="N6" s="17">
+        <v>2</v>
+      </c>
+      <c r="O6" s="18">
+        <v>2</v>
+      </c>
       <c r="P6" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Q6" s="20"/>
       <c r="R6" s="17"/>
@@ -2247,8 +2271,8 @@
         <v>0</v>
       </c>
       <c r="V6" s="21">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="V3:V10" si="4">SUM(U6,P6,F6)</f>
+        <v>6</v>
       </c>
       <c r="W6" s="2"/>
       <c r="X6" s="3"/>
@@ -2264,7 +2288,7 @@
       <c r="D7" s="17"/>
       <c r="E7" s="18"/>
       <c r="F7" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G7" s="20"/>
@@ -2292,7 +2316,7 @@
         <v>0</v>
       </c>
       <c r="V7" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W7" s="2"/>
@@ -2309,7 +2333,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="18"/>
       <c r="F8" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G8" s="20"/>
@@ -2337,7 +2361,7 @@
         <v>0</v>
       </c>
       <c r="V8" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="W8" s="2"/>
@@ -2354,24 +2378,30 @@
       <c r="D9" s="17"/>
       <c r="E9" s="18"/>
       <c r="F9" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
+      <c r="I9" s="17">
+        <v>4</v>
+      </c>
       <c r="J9" s="18"/>
       <c r="K9" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L9" s="20"/>
       <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="18"/>
+      <c r="N9" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="O9" s="18">
+        <v>1</v>
+      </c>
       <c r="P9" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="Q9" s="20"/>
       <c r="R9" s="17"/>
@@ -2382,8 +2412,8 @@
         <v>0</v>
       </c>
       <c r="V9" s="21">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>2.5</v>
       </c>
       <c r="W9" s="2"/>
       <c r="X9" s="3"/>
@@ -2399,7 +2429,7 @@
       <c r="D10" s="25"/>
       <c r="E10" s="26"/>
       <c r="F10" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G10" s="28"/>
@@ -2429,7 +2459,7 @@
         <v>0</v>
       </c>
       <c r="V10" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="W10" s="2"/>
@@ -2467,39 +2497,39 @@
       </c>
       <c r="H11" s="33">
         <f>SUM(H3:H10)</f>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="I11" s="33">
         <f t="shared" si="5"/>
-        <v>0.5</v>
+        <v>7.5</v>
       </c>
       <c r="J11" s="34">
         <f t="shared" si="5"/>
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="K11" s="35">
         <f t="shared" si="5"/>
-        <v>3.5</v>
+        <v>13.5</v>
       </c>
       <c r="L11" s="32">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M11" s="33">
         <f t="shared" si="5"/>
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="N11" s="33">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O11" s="34">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="P11" s="35">
         <f t="shared" si="5"/>
-        <v>0.5</v>
+        <v>11</v>
       </c>
       <c r="Q11" s="32">
         <f t="shared" si="5"/>
@@ -2523,7 +2553,7 @@
       </c>
       <c r="V11" s="36">
         <f t="shared" si="5"/>
-        <v>8.75</v>
+        <v>28.75</v>
       </c>
       <c r="W11" s="2"/>
       <c r="X11" s="3"/>

</xml_diff>